<commit_message>
Add specific items to WBS 4.2
</commit_message>
<xml_diff>
--- a/Phase 2/Project Plan/Project Plan Crawford Long.xlsx
+++ b/Phase 2/Project Plan/Project Plan Crawford Long.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharkPeeler\Documents\Mark's School Stuff\MIST7590\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcritt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11145" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11145" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t>Task or Deliverable - WBS</t>
   </si>
@@ -177,9 +177,6 @@
     <t>4.2  Write the Code</t>
   </si>
   <si>
-    <t>4.2.1 &lt;Enter detailed deliverables&gt;</t>
-  </si>
-  <si>
     <t>4.3  Test the Application</t>
   </si>
   <si>
@@ -257,11 +254,32 @@
   <si>
     <t>Ashley, Justin</t>
   </si>
+  <si>
+    <t>4.2.1 Front End Development</t>
+  </si>
+  <si>
+    <t>4.2.2 Back End Development</t>
+  </si>
+  <si>
+    <t>4.2.3 Integration</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Ben Pitts, Justin Ucol, Ashley Reese</t>
+  </si>
+  <si>
+    <t>Daniel Crittenden, John Peeler, Ashley Reese, Justin Ucol</t>
+  </si>
+  <si>
+    <t>Ashley Reese, John Peeler, Justin Ucol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
@@ -803,14 +821,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AR1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V19" sqref="V19:W19"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -821,7 +839,7 @@
     <col min="5" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="41" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="41" customWidth="1"/>
     <col min="11" max="23" width="7.7109375" customWidth="1"/>
     <col min="24" max="24" width="10.7109375" customWidth="1"/>
     <col min="25" max="32" width="7.7109375" customWidth="1"/>
@@ -1084,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
@@ -1146,7 +1164,7 @@
       <c r="T5" s="18"/>
       <c r="U5" s="18"/>
       <c r="V5" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W5" s="18"/>
       <c r="X5" s="23"/>
@@ -1194,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
@@ -1254,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="22"/>
@@ -1314,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
@@ -1374,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
@@ -1434,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
@@ -1494,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
@@ -1554,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
@@ -1614,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -1765,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -1825,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -1885,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
@@ -1993,7 +2011,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
@@ -2053,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
@@ -2113,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
@@ -2173,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
@@ -2233,7 +2251,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
@@ -2339,7 +2357,7 @@
         <v>0.95</v>
       </c>
       <c r="J26" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
@@ -2397,7 +2415,7 @@
         <v>0.95</v>
       </c>
       <c r="J27" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
@@ -2455,7 +2473,7 @@
         <v>0.9</v>
       </c>
       <c r="J28" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
@@ -2603,7 +2621,7 @@
       <c r="H31" s="20"/>
       <c r="I31" s="21"/>
       <c r="J31" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
@@ -2653,7 +2671,7 @@
       <c r="H32" s="20"/>
       <c r="I32" s="21"/>
       <c r="J32" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
@@ -3314,19 +3332,23 @@
       <c r="AQ45" s="24"/>
       <c r="AR45" s="1"/>
     </row>
-    <row r="46" spans="1:44" ht="15.75">
+    <row r="46" spans="1:44" ht="31.5">
       <c r="A46" s="16"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D46" s="18"/>
-      <c r="E46" s="19"/>
+      <c r="E46" s="19">
+        <v>43103</v>
+      </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
       <c r="H46" s="20"/>
       <c r="I46" s="21"/>
-      <c r="J46" s="39"/>
+      <c r="J46" s="39" t="s">
+        <v>82</v>
+      </c>
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
       <c r="M46" s="18"/>
@@ -3362,19 +3384,23 @@
       <c r="AQ46" s="24"/>
       <c r="AR46" s="1"/>
     </row>
-    <row r="47" spans="1:44" ht="15.75">
+    <row r="47" spans="1:44" ht="47.25">
       <c r="A47" s="16"/>
-      <c r="B47" s="17" t="s">
-        <v>53</v>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17" t="s">
+        <v>79</v>
       </c>
-      <c r="C47" s="17"/>
       <c r="D47" s="18"/>
-      <c r="E47" s="19"/>
+      <c r="E47" s="19">
+        <v>43103</v>
+      </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
       <c r="H47" s="20"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="39"/>
+      <c r="J47" s="39" t="s">
+        <v>83</v>
+      </c>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
       <c r="M47" s="18"/>
@@ -3410,19 +3436,23 @@
       <c r="AQ47" s="24"/>
       <c r="AR47" s="1"/>
     </row>
-    <row r="48" spans="1:44" ht="15.75">
+    <row r="48" spans="1:44" ht="31.5">
       <c r="A48" s="16"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="D48" s="18"/>
-      <c r="E48" s="19"/>
+      <c r="E48" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
       <c r="H48" s="20"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="39"/>
+      <c r="J48" s="39" t="s">
+        <v>84</v>
+      </c>
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
       <c r="M48" s="18"/>
@@ -3448,10 +3478,10 @@
       <c r="AG48" s="25"/>
       <c r="AH48" s="25"/>
       <c r="AI48" s="24"/>
-      <c r="AJ48" s="32"/>
-      <c r="AK48" s="32"/>
-      <c r="AL48" s="32"/>
-      <c r="AM48" s="32"/>
+      <c r="AJ48" s="24"/>
+      <c r="AK48" s="24"/>
+      <c r="AL48" s="24"/>
+      <c r="AM48" s="24"/>
       <c r="AN48" s="24"/>
       <c r="AO48" s="24"/>
       <c r="AP48" s="24"/>
@@ -3460,10 +3490,10 @@
     </row>
     <row r="49" spans="1:44" ht="15.75">
       <c r="A49" s="16"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17" t="s">
-        <v>55</v>
+      <c r="B49" s="17" t="s">
+        <v>52</v>
       </c>
+      <c r="C49" s="17"/>
       <c r="D49" s="18"/>
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
@@ -3496,10 +3526,10 @@
       <c r="AG49" s="25"/>
       <c r="AH49" s="25"/>
       <c r="AI49" s="24"/>
-      <c r="AJ49" s="32"/>
-      <c r="AK49" s="32"/>
-      <c r="AL49" s="32"/>
-      <c r="AM49" s="32"/>
+      <c r="AJ49" s="24"/>
+      <c r="AK49" s="24"/>
+      <c r="AL49" s="24"/>
+      <c r="AM49" s="24"/>
       <c r="AN49" s="24"/>
       <c r="AO49" s="24"/>
       <c r="AP49" s="24"/>
@@ -3510,7 +3540,7 @@
       <c r="A50" s="16"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="19"/>
@@ -3558,7 +3588,7 @@
       <c r="A51" s="16"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D51" s="18"/>
       <c r="E51" s="19"/>
@@ -3604,10 +3634,10 @@
     </row>
     <row r="52" spans="1:44" ht="15.75">
       <c r="A52" s="16"/>
-      <c r="B52" s="17" t="s">
-        <v>58</v>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17" t="s">
+        <v>55</v>
       </c>
-      <c r="C52" s="17"/>
       <c r="D52" s="18"/>
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
@@ -3640,10 +3670,10 @@
       <c r="AG52" s="25"/>
       <c r="AH52" s="25"/>
       <c r="AI52" s="24"/>
-      <c r="AJ52" s="24"/>
-      <c r="AK52" s="24"/>
-      <c r="AL52" s="24"/>
-      <c r="AM52" s="24"/>
+      <c r="AJ52" s="32"/>
+      <c r="AK52" s="32"/>
+      <c r="AL52" s="32"/>
+      <c r="AM52" s="32"/>
       <c r="AN52" s="24"/>
       <c r="AO52" s="24"/>
       <c r="AP52" s="24"/>
@@ -3651,11 +3681,11 @@
       <c r="AR52" s="1"/>
     </row>
     <row r="53" spans="1:44" ht="15.75">
-      <c r="A53" s="16" t="s">
-        <v>59</v>
+      <c r="A53" s="16"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17" t="s">
+        <v>56</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
       <c r="D53" s="18"/>
       <c r="E53" s="19"/>
       <c r="F53" s="19"/>
@@ -3688,20 +3718,20 @@
       <c r="AG53" s="25"/>
       <c r="AH53" s="25"/>
       <c r="AI53" s="24"/>
-      <c r="AJ53" s="24"/>
-      <c r="AK53" s="24"/>
-      <c r="AL53" s="33"/>
-      <c r="AM53" s="33"/>
-      <c r="AN53" s="33"/>
-      <c r="AO53" s="33"/>
-      <c r="AP53" s="33"/>
-      <c r="AQ53" s="33"/>
+      <c r="AJ53" s="32"/>
+      <c r="AK53" s="32"/>
+      <c r="AL53" s="32"/>
+      <c r="AM53" s="32"/>
+      <c r="AN53" s="24"/>
+      <c r="AO53" s="24"/>
+      <c r="AP53" s="24"/>
+      <c r="AQ53" s="24"/>
       <c r="AR53" s="1"/>
     </row>
     <row r="54" spans="1:44" ht="15.75">
       <c r="A54" s="16"/>
       <c r="B54" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C54" s="17"/>
       <c r="D54" s="18"/>
@@ -3738,8 +3768,8 @@
       <c r="AI54" s="24"/>
       <c r="AJ54" s="24"/>
       <c r="AK54" s="24"/>
-      <c r="AL54" s="33"/>
-      <c r="AM54" s="33"/>
+      <c r="AL54" s="24"/>
+      <c r="AM54" s="24"/>
       <c r="AN54" s="24"/>
       <c r="AO54" s="24"/>
       <c r="AP54" s="24"/>
@@ -3747,10 +3777,10 @@
       <c r="AR54" s="1"/>
     </row>
     <row r="55" spans="1:44" ht="15.75">
-      <c r="A55" s="16"/>
-      <c r="B55" s="17" t="s">
-        <v>61</v>
+      <c r="A55" s="16" t="s">
+        <v>58</v>
       </c>
+      <c r="B55" s="17"/>
       <c r="C55" s="17"/>
       <c r="D55" s="18"/>
       <c r="E55" s="19"/>
@@ -3786,18 +3816,18 @@
       <c r="AI55" s="24"/>
       <c r="AJ55" s="24"/>
       <c r="AK55" s="24"/>
-      <c r="AL55" s="24"/>
+      <c r="AL55" s="33"/>
       <c r="AM55" s="33"/>
       <c r="AN55" s="33"/>
       <c r="AO55" s="33"/>
       <c r="AP55" s="33"/>
-      <c r="AQ55" s="24"/>
+      <c r="AQ55" s="33"/>
       <c r="AR55" s="1"/>
     </row>
     <row r="56" spans="1:44" ht="15.75">
       <c r="A56" s="16"/>
       <c r="B56" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="18"/>
@@ -3834,20 +3864,20 @@
       <c r="AI56" s="24"/>
       <c r="AJ56" s="24"/>
       <c r="AK56" s="24"/>
-      <c r="AL56" s="24"/>
-      <c r="AM56" s="24"/>
+      <c r="AL56" s="33"/>
+      <c r="AM56" s="33"/>
       <c r="AN56" s="24"/>
-      <c r="AO56" s="25"/>
-      <c r="AP56" s="25"/>
-      <c r="AQ56" s="33"/>
+      <c r="AO56" s="24"/>
+      <c r="AP56" s="24"/>
+      <c r="AQ56" s="24"/>
       <c r="AR56" s="1"/>
     </row>
     <row r="57" spans="1:44" ht="15.75">
       <c r="A57" s="16"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17" t="s">
-        <v>63</v>
+      <c r="B57" s="17" t="s">
+        <v>60</v>
       </c>
+      <c r="C57" s="17"/>
       <c r="D57" s="18"/>
       <c r="E57" s="19"/>
       <c r="F57" s="19"/>
@@ -3883,19 +3913,19 @@
       <c r="AJ57" s="24"/>
       <c r="AK57" s="24"/>
       <c r="AL57" s="24"/>
-      <c r="AM57" s="24"/>
-      <c r="AN57" s="24"/>
-      <c r="AO57" s="24"/>
+      <c r="AM57" s="33"/>
+      <c r="AN57" s="33"/>
+      <c r="AO57" s="33"/>
       <c r="AP57" s="33"/>
       <c r="AQ57" s="24"/>
       <c r="AR57" s="1"/>
     </row>
     <row r="58" spans="1:44" ht="15.75">
       <c r="A58" s="16"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17" t="s">
-        <v>64</v>
+      <c r="B58" s="17" t="s">
+        <v>61</v>
       </c>
+      <c r="C58" s="17"/>
       <c r="D58" s="18"/>
       <c r="E58" s="19"/>
       <c r="F58" s="19"/>
@@ -3933,17 +3963,17 @@
       <c r="AL58" s="24"/>
       <c r="AM58" s="24"/>
       <c r="AN58" s="24"/>
-      <c r="AO58" s="24"/>
-      <c r="AP58" s="24"/>
+      <c r="AO58" s="25"/>
+      <c r="AP58" s="25"/>
       <c r="AQ58" s="33"/>
       <c r="AR58" s="1"/>
     </row>
     <row r="59" spans="1:44" ht="15.75">
-      <c r="A59" s="16" t="s">
-        <v>65</v>
+      <c r="A59" s="16"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17" t="s">
+        <v>62</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
       <c r="D59" s="18"/>
       <c r="E59" s="19"/>
       <c r="F59" s="19"/>
@@ -3953,45 +3983,45 @@
       <c r="J59" s="39"/>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
-      <c r="M59" s="34"/>
-      <c r="N59" s="34"/>
-      <c r="O59" s="34"/>
-      <c r="P59" s="34"/>
-      <c r="Q59" s="34"/>
-      <c r="R59" s="34"/>
-      <c r="S59" s="34"/>
-      <c r="T59" s="34"/>
-      <c r="U59" s="34"/>
-      <c r="V59" s="34"/>
-      <c r="W59" s="34"/>
-      <c r="X59" s="35"/>
-      <c r="Y59" s="36"/>
-      <c r="Z59" s="36"/>
-      <c r="AA59" s="36"/>
-      <c r="AB59" s="36"/>
-      <c r="AC59" s="36"/>
-      <c r="AD59" s="36"/>
-      <c r="AE59" s="36"/>
-      <c r="AF59" s="36"/>
-      <c r="AG59" s="36"/>
-      <c r="AH59" s="36"/>
-      <c r="AI59" s="36"/>
-      <c r="AJ59" s="36"/>
-      <c r="AK59" s="36"/>
-      <c r="AL59" s="36"/>
-      <c r="AM59" s="36"/>
-      <c r="AN59" s="36"/>
-      <c r="AO59" s="36"/>
-      <c r="AP59" s="36"/>
-      <c r="AQ59" s="36"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="18"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" s="18"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="18"/>
+      <c r="U59" s="18"/>
+      <c r="V59" s="18"/>
+      <c r="W59" s="18"/>
+      <c r="X59" s="23"/>
+      <c r="Y59" s="24"/>
+      <c r="Z59" s="24"/>
+      <c r="AA59" s="24"/>
+      <c r="AB59" s="24"/>
+      <c r="AC59" s="24"/>
+      <c r="AD59" s="24"/>
+      <c r="AE59" s="24"/>
+      <c r="AF59" s="24"/>
+      <c r="AG59" s="25"/>
+      <c r="AH59" s="25"/>
+      <c r="AI59" s="24"/>
+      <c r="AJ59" s="24"/>
+      <c r="AK59" s="24"/>
+      <c r="AL59" s="24"/>
+      <c r="AM59" s="24"/>
+      <c r="AN59" s="24"/>
+      <c r="AO59" s="24"/>
+      <c r="AP59" s="33"/>
+      <c r="AQ59" s="24"/>
       <c r="AR59" s="1"/>
     </row>
     <row r="60" spans="1:44" ht="15.75">
       <c r="A60" s="16"/>
-      <c r="B60" s="17" t="s">
-        <v>66</v>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17" t="s">
+        <v>63</v>
       </c>
-      <c r="C60" s="17"/>
       <c r="D60" s="18"/>
       <c r="E60" s="19"/>
       <c r="F60" s="19"/>
@@ -4027,18 +4057,18 @@
       <c r="AJ60" s="24"/>
       <c r="AK60" s="24"/>
       <c r="AL60" s="24"/>
-      <c r="AM60" s="36"/>
-      <c r="AN60" s="36"/>
-      <c r="AO60" s="36"/>
+      <c r="AM60" s="24"/>
+      <c r="AN60" s="24"/>
+      <c r="AO60" s="24"/>
       <c r="AP60" s="24"/>
-      <c r="AQ60" s="24"/>
+      <c r="AQ60" s="33"/>
       <c r="AR60" s="1"/>
     </row>
     <row r="61" spans="1:44" ht="15.75">
-      <c r="A61" s="16"/>
-      <c r="B61" s="17" t="s">
-        <v>67</v>
+      <c r="A61" s="16" t="s">
+        <v>64</v>
       </c>
+      <c r="B61" s="17"/>
       <c r="C61" s="17"/>
       <c r="D61" s="18"/>
       <c r="E61" s="19"/>
@@ -4049,45 +4079,45 @@
       <c r="J61" s="39"/>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
-      <c r="M61" s="18"/>
-      <c r="N61" s="18"/>
-      <c r="O61" s="18"/>
-      <c r="P61" s="18"/>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-      <c r="S61" s="18"/>
-      <c r="T61" s="18"/>
-      <c r="U61" s="18"/>
-      <c r="V61" s="18"/>
-      <c r="W61" s="18"/>
-      <c r="X61" s="23"/>
-      <c r="Y61" s="24"/>
-      <c r="Z61" s="24"/>
-      <c r="AA61" s="24"/>
-      <c r="AB61" s="24"/>
-      <c r="AC61" s="24"/>
-      <c r="AD61" s="24"/>
-      <c r="AE61" s="24"/>
-      <c r="AF61" s="24"/>
-      <c r="AG61" s="25"/>
-      <c r="AH61" s="25"/>
-      <c r="AI61" s="24"/>
-      <c r="AJ61" s="24"/>
-      <c r="AK61" s="24"/>
-      <c r="AL61" s="24"/>
-      <c r="AM61" s="24"/>
-      <c r="AN61" s="24"/>
-      <c r="AO61" s="24"/>
-      <c r="AP61" s="24"/>
-      <c r="AQ61" s="24"/>
+      <c r="M61" s="34"/>
+      <c r="N61" s="34"/>
+      <c r="O61" s="34"/>
+      <c r="P61" s="34"/>
+      <c r="Q61" s="34"/>
+      <c r="R61" s="34"/>
+      <c r="S61" s="34"/>
+      <c r="T61" s="34"/>
+      <c r="U61" s="34"/>
+      <c r="V61" s="34"/>
+      <c r="W61" s="34"/>
+      <c r="X61" s="35"/>
+      <c r="Y61" s="36"/>
+      <c r="Z61" s="36"/>
+      <c r="AA61" s="36"/>
+      <c r="AB61" s="36"/>
+      <c r="AC61" s="36"/>
+      <c r="AD61" s="36"/>
+      <c r="AE61" s="36"/>
+      <c r="AF61" s="36"/>
+      <c r="AG61" s="36"/>
+      <c r="AH61" s="36"/>
+      <c r="AI61" s="36"/>
+      <c r="AJ61" s="36"/>
+      <c r="AK61" s="36"/>
+      <c r="AL61" s="36"/>
+      <c r="AM61" s="36"/>
+      <c r="AN61" s="36"/>
+      <c r="AO61" s="36"/>
+      <c r="AP61" s="36"/>
+      <c r="AQ61" s="36"/>
       <c r="AR61" s="1"/>
     </row>
     <row r="62" spans="1:44" ht="15.75">
       <c r="A62" s="16"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17" t="s">
-        <v>68</v>
+      <c r="B62" s="17" t="s">
+        <v>65</v>
       </c>
+      <c r="C62" s="17"/>
       <c r="D62" s="18"/>
       <c r="E62" s="19"/>
       <c r="F62" s="19"/>
@@ -4097,18 +4127,18 @@
       <c r="J62" s="39"/>
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
-      <c r="M62" s="34"/>
-      <c r="N62" s="34"/>
-      <c r="O62" s="34"/>
-      <c r="P62" s="34"/>
-      <c r="Q62" s="34"/>
-      <c r="R62" s="34"/>
-      <c r="S62" s="34"/>
-      <c r="T62" s="34"/>
-      <c r="U62" s="34"/>
-      <c r="V62" s="34"/>
-      <c r="W62" s="34"/>
-      <c r="X62" s="35"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" s="18"/>
+      <c r="S62" s="18"/>
+      <c r="T62" s="18"/>
+      <c r="U62" s="18"/>
+      <c r="V62" s="18"/>
+      <c r="W62" s="18"/>
+      <c r="X62" s="23"/>
       <c r="Y62" s="24"/>
       <c r="Z62" s="24"/>
       <c r="AA62" s="24"/>
@@ -4123,19 +4153,19 @@
       <c r="AJ62" s="24"/>
       <c r="AK62" s="24"/>
       <c r="AL62" s="24"/>
-      <c r="AM62" s="24"/>
-      <c r="AN62" s="24"/>
-      <c r="AO62" s="24"/>
+      <c r="AM62" s="36"/>
+      <c r="AN62" s="36"/>
+      <c r="AO62" s="36"/>
       <c r="AP62" s="24"/>
       <c r="AQ62" s="24"/>
       <c r="AR62" s="1"/>
     </row>
     <row r="63" spans="1:44" ht="15.75">
       <c r="A63" s="16"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17" t="s">
-        <v>69</v>
+      <c r="B63" s="17" t="s">
+        <v>66</v>
       </c>
+      <c r="C63" s="17"/>
       <c r="D63" s="18"/>
       <c r="E63" s="19"/>
       <c r="F63" s="19"/>
@@ -4157,24 +4187,24 @@
       <c r="V63" s="18"/>
       <c r="W63" s="18"/>
       <c r="X63" s="23"/>
-      <c r="Y63" s="36"/>
-      <c r="Z63" s="36"/>
-      <c r="AA63" s="36"/>
-      <c r="AB63" s="36"/>
-      <c r="AC63" s="36"/>
-      <c r="AD63" s="36"/>
-      <c r="AE63" s="36"/>
-      <c r="AF63" s="36"/>
-      <c r="AG63" s="36"/>
-      <c r="AH63" s="36"/>
-      <c r="AI63" s="36"/>
-      <c r="AJ63" s="36"/>
-      <c r="AK63" s="36"/>
-      <c r="AL63" s="36"/>
-      <c r="AM63" s="36"/>
-      <c r="AN63" s="36"/>
-      <c r="AO63" s="36"/>
-      <c r="AP63" s="36"/>
+      <c r="Y63" s="24"/>
+      <c r="Z63" s="24"/>
+      <c r="AA63" s="24"/>
+      <c r="AB63" s="24"/>
+      <c r="AC63" s="24"/>
+      <c r="AD63" s="24"/>
+      <c r="AE63" s="24"/>
+      <c r="AF63" s="24"/>
+      <c r="AG63" s="25"/>
+      <c r="AH63" s="25"/>
+      <c r="AI63" s="24"/>
+      <c r="AJ63" s="24"/>
+      <c r="AK63" s="24"/>
+      <c r="AL63" s="24"/>
+      <c r="AM63" s="24"/>
+      <c r="AN63" s="24"/>
+      <c r="AO63" s="24"/>
+      <c r="AP63" s="24"/>
       <c r="AQ63" s="24"/>
       <c r="AR63" s="1"/>
     </row>
@@ -4182,7 +4212,7 @@
       <c r="A64" s="16"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D64" s="18"/>
       <c r="E64" s="19"/>
@@ -4193,18 +4223,18 @@
       <c r="J64" s="39"/>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
-      <c r="M64" s="18"/>
-      <c r="N64" s="18"/>
-      <c r="O64" s="18"/>
-      <c r="P64" s="18"/>
-      <c r="Q64" s="18"/>
-      <c r="R64" s="18"/>
-      <c r="S64" s="18"/>
-      <c r="T64" s="18"/>
-      <c r="U64" s="18"/>
-      <c r="V64" s="18"/>
-      <c r="W64" s="18"/>
-      <c r="X64" s="23"/>
+      <c r="M64" s="34"/>
+      <c r="N64" s="34"/>
+      <c r="O64" s="34"/>
+      <c r="P64" s="34"/>
+      <c r="Q64" s="34"/>
+      <c r="R64" s="34"/>
+      <c r="S64" s="34"/>
+      <c r="T64" s="34"/>
+      <c r="U64" s="34"/>
+      <c r="V64" s="34"/>
+      <c r="W64" s="34"/>
+      <c r="X64" s="35"/>
       <c r="Y64" s="24"/>
       <c r="Z64" s="24"/>
       <c r="AA64" s="24"/>
@@ -4221,15 +4251,17 @@
       <c r="AL64" s="24"/>
       <c r="AM64" s="24"/>
       <c r="AN64" s="24"/>
-      <c r="AO64" s="36"/>
-      <c r="AP64" s="36"/>
-      <c r="AQ64" s="36"/>
+      <c r="AO64" s="24"/>
+      <c r="AP64" s="24"/>
+      <c r="AQ64" s="24"/>
       <c r="AR64" s="1"/>
     </row>
     <row r="65" spans="1:44" ht="15.75">
       <c r="A65" s="16"/>
       <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
+      <c r="C65" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="D65" s="18"/>
       <c r="E65" s="19"/>
       <c r="F65" s="19"/>
@@ -4251,117 +4283,119 @@
       <c r="V65" s="18"/>
       <c r="W65" s="18"/>
       <c r="X65" s="23"/>
-      <c r="Y65" s="24"/>
-      <c r="Z65" s="24"/>
-      <c r="AA65" s="24"/>
-      <c r="AB65" s="24"/>
-      <c r="AC65" s="24"/>
-      <c r="AD65" s="24"/>
-      <c r="AE65" s="24"/>
-      <c r="AF65" s="24"/>
-      <c r="AG65" s="25"/>
-      <c r="AH65" s="25"/>
-      <c r="AI65" s="24"/>
-      <c r="AJ65" s="24"/>
-      <c r="AK65" s="24"/>
-      <c r="AL65" s="24"/>
-      <c r="AM65" s="24"/>
-      <c r="AN65" s="24"/>
-      <c r="AO65" s="24"/>
-      <c r="AP65" s="24"/>
+      <c r="Y65" s="36"/>
+      <c r="Z65" s="36"/>
+      <c r="AA65" s="36"/>
+      <c r="AB65" s="36"/>
+      <c r="AC65" s="36"/>
+      <c r="AD65" s="36"/>
+      <c r="AE65" s="36"/>
+      <c r="AF65" s="36"/>
+      <c r="AG65" s="36"/>
+      <c r="AH65" s="36"/>
+      <c r="AI65" s="36"/>
+      <c r="AJ65" s="36"/>
+      <c r="AK65" s="36"/>
+      <c r="AL65" s="36"/>
+      <c r="AM65" s="36"/>
+      <c r="AN65" s="36"/>
+      <c r="AO65" s="36"/>
+      <c r="AP65" s="36"/>
       <c r="AQ65" s="24"/>
       <c r="AR65" s="1"/>
     </row>
     <row r="66" spans="1:44" ht="15.75">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="40"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
-      <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
-      <c r="V66" s="1"/>
-      <c r="W66" s="1"/>
-      <c r="X66" s="37"/>
-      <c r="Y66" s="1"/>
-      <c r="Z66" s="1"/>
-      <c r="AA66" s="1"/>
-      <c r="AB66" s="1"/>
-      <c r="AC66" s="1"/>
-      <c r="AD66" s="1"/>
-      <c r="AE66" s="1"/>
-      <c r="AF66" s="1"/>
-      <c r="AG66" s="38"/>
-      <c r="AH66" s="38"/>
-      <c r="AI66" s="1"/>
-      <c r="AJ66" s="1"/>
-      <c r="AK66" s="1"/>
-      <c r="AL66" s="1"/>
-      <c r="AM66" s="1"/>
-      <c r="AN66" s="1"/>
-      <c r="AO66" s="1"/>
-      <c r="AP66" s="1"/>
-      <c r="AQ66" s="1"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" s="18"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="39"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="18"/>
+      <c r="Q66" s="18"/>
+      <c r="R66" s="18"/>
+      <c r="S66" s="18"/>
+      <c r="T66" s="18"/>
+      <c r="U66" s="18"/>
+      <c r="V66" s="18"/>
+      <c r="W66" s="18"/>
+      <c r="X66" s="23"/>
+      <c r="Y66" s="24"/>
+      <c r="Z66" s="24"/>
+      <c r="AA66" s="24"/>
+      <c r="AB66" s="24"/>
+      <c r="AC66" s="24"/>
+      <c r="AD66" s="24"/>
+      <c r="AE66" s="24"/>
+      <c r="AF66" s="24"/>
+      <c r="AG66" s="25"/>
+      <c r="AH66" s="25"/>
+      <c r="AI66" s="24"/>
+      <c r="AJ66" s="24"/>
+      <c r="AK66" s="24"/>
+      <c r="AL66" s="24"/>
+      <c r="AM66" s="24"/>
+      <c r="AN66" s="24"/>
+      <c r="AO66" s="36"/>
+      <c r="AP66" s="36"/>
+      <c r="AQ66" s="36"/>
       <c r="AR66" s="1"/>
     </row>
     <row r="67" spans="1:44" ht="15.75">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="40"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="37"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-      <c r="AE67" s="1"/>
-      <c r="AF67" s="1"/>
-      <c r="AG67" s="38"/>
-      <c r="AH67" s="38"/>
-      <c r="AI67" s="1"/>
-      <c r="AJ67" s="1"/>
-      <c r="AK67" s="1"/>
-      <c r="AL67" s="1"/>
-      <c r="AM67" s="1"/>
-      <c r="AN67" s="1"/>
-      <c r="AO67" s="1"/>
-      <c r="AP67" s="1"/>
-      <c r="AQ67" s="1"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="39"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="18"/>
+      <c r="R67" s="18"/>
+      <c r="S67" s="18"/>
+      <c r="T67" s="18"/>
+      <c r="U67" s="18"/>
+      <c r="V67" s="18"/>
+      <c r="W67" s="18"/>
+      <c r="X67" s="23"/>
+      <c r="Y67" s="24"/>
+      <c r="Z67" s="24"/>
+      <c r="AA67" s="24"/>
+      <c r="AB67" s="24"/>
+      <c r="AC67" s="24"/>
+      <c r="AD67" s="24"/>
+      <c r="AE67" s="24"/>
+      <c r="AF67" s="24"/>
+      <c r="AG67" s="25"/>
+      <c r="AH67" s="25"/>
+      <c r="AI67" s="24"/>
+      <c r="AJ67" s="24"/>
+      <c r="AK67" s="24"/>
+      <c r="AL67" s="24"/>
+      <c r="AM67" s="24"/>
+      <c r="AN67" s="24"/>
+      <c r="AO67" s="24"/>
+      <c r="AP67" s="24"/>
+      <c r="AQ67" s="24"/>
       <c r="AR67" s="1"/>
     </row>
     <row r="68" spans="1:44" ht="15.75">
@@ -47282,6 +47316,98 @@
       <c r="AQ1000" s="1"/>
       <c r="AR1000" s="1"/>
     </row>
+    <row r="1001" spans="1:44" ht="15.75">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+      <c r="G1001" s="1"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="40"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="37"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+      <c r="AA1001" s="1"/>
+      <c r="AB1001" s="1"/>
+      <c r="AC1001" s="1"/>
+      <c r="AD1001" s="1"/>
+      <c r="AE1001" s="1"/>
+      <c r="AF1001" s="1"/>
+      <c r="AG1001" s="38"/>
+      <c r="AH1001" s="38"/>
+      <c r="AI1001" s="1"/>
+      <c r="AJ1001" s="1"/>
+      <c r="AK1001" s="1"/>
+      <c r="AL1001" s="1"/>
+      <c r="AM1001" s="1"/>
+      <c r="AN1001" s="1"/>
+      <c r="AO1001" s="1"/>
+      <c r="AP1001" s="1"/>
+      <c r="AQ1001" s="1"/>
+      <c r="AR1001" s="1"/>
+    </row>
+    <row r="1002" spans="1:44" ht="15.75">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="40"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="37"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+      <c r="AA1002" s="1"/>
+      <c r="AB1002" s="1"/>
+      <c r="AC1002" s="1"/>
+      <c r="AD1002" s="1"/>
+      <c r="AE1002" s="1"/>
+      <c r="AF1002" s="1"/>
+      <c r="AG1002" s="38"/>
+      <c r="AH1002" s="38"/>
+      <c r="AI1002" s="1"/>
+      <c r="AJ1002" s="1"/>
+      <c r="AK1002" s="1"/>
+      <c r="AL1002" s="1"/>
+      <c r="AM1002" s="1"/>
+      <c r="AN1002" s="1"/>
+      <c r="AO1002" s="1"/>
+      <c r="AP1002" s="1"/>
+      <c r="AQ1002" s="1"/>
+      <c r="AR1002" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="Y1:AH1"/>

</xml_diff>

<commit_message>
Minor tweaks to project plan
</commit_message>
<xml_diff>
--- a/Phase 2/Project Plan/Project Plan Crawford Long.xlsx
+++ b/Phase 2/Project Plan/Project Plan Crawford Long.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcrittenden/Library/Mobile Documents/com~apple~CloudDocs/EPAP/EPAP-Documentation/Phase 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcrittenden/Library/Mobile Documents/com~apple~CloudDocs/EPAP/EPAP-Documentation/Phase 2/Project Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31160" windowHeight="19560"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31160" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="152">
   <si>
     <t>Task or Deliverable - WBS</t>
   </si>
@@ -476,18 +476,15 @@
   <si>
     <t>4.2.8.1.2.2 View open transfer plan requests sent (don’t show accepted/rejected)</t>
   </si>
-  <si>
-    <t>If time available</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -507,6 +504,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -635,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -708,10 +712,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -721,6 +721,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="7"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,14 +1040,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR1068"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J97" sqref="J97"/>
+      <selection pane="bottomRight" activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1096,18 +1102,18 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="4"/>
-      <c r="Y1" s="42">
+      <c r="Y1" s="45">
         <v>2018</v>
       </c>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="43"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
       <c r="AK1" s="5"/>
@@ -3611,7 +3617,7 @@
       <c r="B45" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="17"/>
+      <c r="C45" s="47"/>
       <c r="D45" s="18"/>
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
@@ -3657,13 +3663,13 @@
     <row r="46" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="17"/>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="47" t="s">
         <v>83</v>
       </c>
       <c r="D46" s="18"/>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
-      <c r="G46" s="19">
+      <c r="G46" s="48">
         <v>43131</v>
       </c>
       <c r="H46" s="20"/>
@@ -3851,13 +3857,13 @@
     <row r="50" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="16"/>
       <c r="B50" s="17"/>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="47" t="s">
         <v>93</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
-      <c r="G50" s="19">
+      <c r="G50" s="48">
         <v>43138</v>
       </c>
       <c r="H50" s="20"/>
@@ -4045,13 +4051,13 @@
     <row r="54" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="16"/>
       <c r="B54" s="17"/>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="47" t="s">
         <v>94</v>
       </c>
       <c r="D54" s="18"/>
       <c r="E54" s="19"/>
       <c r="F54" s="19"/>
-      <c r="G54" s="19">
+      <c r="G54" s="48">
         <v>43145</v>
       </c>
       <c r="H54" s="20"/>
@@ -4239,14 +4245,14 @@
     <row r="58" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="16"/>
       <c r="B58" s="17"/>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="47" t="s">
         <v>95</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="19"/>
       <c r="F58" s="19"/>
-      <c r="G58" s="19">
-        <v>43152</v>
+      <c r="G58" s="48">
+        <v>43159</v>
       </c>
       <c r="H58" s="20"/>
       <c r="I58" s="21"/>
@@ -4295,7 +4301,9 @@
       </c>
       <c r="E59" s="19"/>
       <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
+      <c r="G59" s="19">
+        <v>43152</v>
+      </c>
       <c r="H59" s="20"/>
       <c r="I59" s="21"/>
       <c r="J59" s="39"/>
@@ -4631,7 +4639,9 @@
       </c>
       <c r="E66" s="19"/>
       <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
+      <c r="G66" s="19">
+        <v>43152</v>
+      </c>
       <c r="H66" s="20"/>
       <c r="I66" s="21"/>
       <c r="J66" s="39"/>
@@ -4823,7 +4833,9 @@
       </c>
       <c r="E70" s="19"/>
       <c r="F70" s="19"/>
-      <c r="G70" s="19"/>
+      <c r="G70" s="19">
+        <v>43159</v>
+      </c>
       <c r="H70" s="20"/>
       <c r="I70" s="21"/>
       <c r="J70" s="39"/>
@@ -5111,7 +5123,9 @@
       </c>
       <c r="E76" s="19"/>
       <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
+      <c r="G76" s="19">
+        <v>43159</v>
+      </c>
       <c r="H76" s="20"/>
       <c r="I76" s="21"/>
       <c r="J76" s="39"/>
@@ -5159,7 +5173,9 @@
       </c>
       <c r="E77" s="19"/>
       <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
+      <c r="G77" s="19">
+        <v>43159</v>
+      </c>
       <c r="H77" s="20"/>
       <c r="I77" s="21"/>
       <c r="J77" s="39"/>
@@ -5297,14 +5313,14 @@
     <row r="80" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="16"/>
       <c r="B80" s="17"/>
-      <c r="C80" s="17" t="s">
+      <c r="C80" s="47" t="s">
         <v>122</v>
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="19"/>
       <c r="F80" s="19"/>
-      <c r="G80" s="19">
-        <v>43159</v>
+      <c r="G80" s="48">
+        <v>43166</v>
       </c>
       <c r="H80" s="20"/>
       <c r="I80" s="21"/>
@@ -5635,14 +5651,14 @@
     <row r="87" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="16"/>
       <c r="B87" s="17"/>
-      <c r="C87" s="17" t="s">
+      <c r="C87" s="47" t="s">
         <v>123</v>
       </c>
       <c r="D87" s="18"/>
       <c r="E87" s="19"/>
       <c r="F87" s="19"/>
-      <c r="G87" s="19">
-        <v>43166</v>
+      <c r="G87" s="48">
+        <v>43173</v>
       </c>
       <c r="H87" s="20"/>
       <c r="I87" s="21"/>
@@ -5734,7 +5750,7 @@
       <c r="A89" s="16"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
-      <c r="D89" s="44" t="s">
+      <c r="D89" s="42" t="s">
         <v>125</v>
       </c>
       <c r="E89" s="19"/>
@@ -5782,7 +5798,7 @@
       <c r="A90" s="16"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
-      <c r="D90" s="44" t="s">
+      <c r="D90" s="42" t="s">
         <v>126</v>
       </c>
       <c r="E90" s="19"/>
@@ -5830,7 +5846,7 @@
       <c r="A91" s="16"/>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
-      <c r="D91" s="44" t="s">
+      <c r="D91" s="42" t="s">
         <v>127</v>
       </c>
       <c r="E91" s="19"/>
@@ -5926,7 +5942,7 @@
       <c r="A93" s="16"/>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
-      <c r="D93" s="44" t="s">
+      <c r="D93" s="42" t="s">
         <v>129</v>
       </c>
       <c r="E93" s="19"/>
@@ -5974,7 +5990,7 @@
       <c r="A94" s="16"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
-      <c r="D94" s="44" t="s">
+      <c r="D94" s="42" t="s">
         <v>130</v>
       </c>
       <c r="E94" s="19"/>
@@ -6213,14 +6229,14 @@
     <row r="99" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="16"/>
       <c r="B99" s="17"/>
-      <c r="C99" s="17" t="s">
+      <c r="C99" s="47" t="s">
         <v>136</v>
       </c>
       <c r="D99" s="18"/>
       <c r="E99" s="19"/>
       <c r="F99" s="19"/>
-      <c r="G99" s="19">
-        <v>43173</v>
+      <c r="G99" s="48">
+        <v>43180</v>
       </c>
       <c r="H99" s="20"/>
       <c r="I99" s="21"/>
@@ -6407,14 +6423,14 @@
     <row r="103" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="16"/>
       <c r="B103" s="17"/>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="47" t="s">
         <v>140</v>
       </c>
       <c r="D103" s="18"/>
       <c r="E103" s="19"/>
       <c r="F103" s="19"/>
-      <c r="G103" s="19" t="s">
-        <v>152</v>
+      <c r="G103" s="48">
+        <v>43187</v>
       </c>
       <c r="H103" s="20"/>
       <c r="I103" s="21"/>
@@ -6506,7 +6522,7 @@
       <c r="A105" s="16"/>
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
-      <c r="D105" s="45" t="s">
+      <c r="D105" s="43" t="s">
         <v>145</v>
       </c>
       <c r="E105" s="19"/>
@@ -6554,7 +6570,7 @@
       <c r="A106" s="16"/>
       <c r="B106" s="17"/>
       <c r="C106" s="17"/>
-      <c r="D106" s="45" t="s">
+      <c r="D106" s="43" t="s">
         <v>142</v>
       </c>
       <c r="E106" s="19"/>
@@ -6602,7 +6618,7 @@
       <c r="A107" s="16"/>
       <c r="B107" s="17"/>
       <c r="C107" s="17"/>
-      <c r="D107" s="46" t="s">
+      <c r="D107" s="44" t="s">
         <v>150</v>
       </c>
       <c r="E107" s="19"/>
@@ -6650,7 +6666,7 @@
       <c r="A108" s="16"/>
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
-      <c r="D108" s="46" t="s">
+      <c r="D108" s="44" t="s">
         <v>151</v>
       </c>
       <c r="E108" s="19"/>
@@ -6698,7 +6714,7 @@
       <c r="A109" s="16"/>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
-      <c r="D109" s="45" t="s">
+      <c r="D109" s="43" t="s">
         <v>143</v>
       </c>
       <c r="E109" s="19"/>
@@ -6746,7 +6762,7 @@
       <c r="A110" s="16"/>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>
-      <c r="D110" s="45" t="s">
+      <c r="D110" s="43" t="s">
         <v>144</v>
       </c>
       <c r="E110" s="19"/>
@@ -6842,7 +6858,7 @@
       <c r="A112" s="16"/>
       <c r="B112" s="17"/>
       <c r="C112" s="17"/>
-      <c r="D112" s="45" t="s">
+      <c r="D112" s="43" t="s">
         <v>147</v>
       </c>
       <c r="E112" s="19"/>
@@ -6890,7 +6906,7 @@
       <c r="A113" s="16"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
-      <c r="D113" s="45" t="s">
+      <c r="D113" s="43" t="s">
         <v>148</v>
       </c>
       <c r="E113" s="19"/>
@@ -6938,7 +6954,7 @@
       <c r="A114" s="16"/>
       <c r="B114" s="17"/>
       <c r="C114" s="17"/>
-      <c r="D114" s="45" t="s">
+      <c r="D114" s="43" t="s">
         <v>149</v>
       </c>
       <c r="E114" s="19"/>

</xml_diff>